<commit_message>
Organização de códigos de exemplo para importação de dados de XLS para SQL Server
</commit_message>
<xml_diff>
--- a/data/sprint_schedules.xlsx
+++ b/data/sprint_schedules.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\FastHTMLcurso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python_Models2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B61672-0AC5-4FAD-8568-1E7F04BC7DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B212BE8B-69EE-462B-95C5-BC66E0DF5367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F5583670-12E1-4BD6-A5F2-68B02C1D08BA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>tDescript</t>
   </si>
@@ -42,51 +42,27 @@
     <t>dPre_sprint_backlog_date</t>
   </si>
   <si>
-    <t>'2024-08-12'</t>
-  </si>
-  <si>
     <t>dScope_start_date</t>
   </si>
   <si>
-    <t>'2024-08-26'</t>
-  </si>
-  <si>
     <t>dScope_approval_date</t>
   </si>
   <si>
-    <t>'2024-09-12'</t>
-  </si>
-  <si>
     <t>dRefinement_date</t>
   </si>
   <si>
-    <t>'2024-09-25'</t>
-  </si>
-  <si>
     <t>dSprint_start_date</t>
   </si>
   <si>
-    <t>'2024-10-11'</t>
-  </si>
-  <si>
     <t>dSprint_end_date</t>
   </si>
   <si>
-    <t>'2024-10-24'</t>
-  </si>
-  <si>
     <t>dSprint_review_date</t>
   </si>
   <si>
-    <t>'2024-10-25'</t>
-  </si>
-  <si>
     <t>tWeek_day</t>
   </si>
   <si>
-    <t>'Friday'</t>
-  </si>
-  <si>
     <t>iBusiness_days</t>
   </si>
   <si>
@@ -96,20 +72,65 @@
     <t>iProjectid</t>
   </si>
   <si>
-    <t>'Sprint 12'</t>
-  </si>
-  <si>
-    <t>'Sprint 13'</t>
-  </si>
-  <si>
-    <t>'Sprint 14'</t>
+    <t xml:space="preserve">Quinta </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sexta </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Terça </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quinta </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Segunda </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quarta </t>
+  </si>
+  <si>
+    <t>Sprint 10</t>
+  </si>
+  <si>
+    <t>Sprint 11</t>
+  </si>
+  <si>
+    <t>Sprint 12</t>
+  </si>
+  <si>
+    <t>Sprint 13</t>
+  </si>
+  <si>
+    <t>Sprint 14</t>
+  </si>
+  <si>
+    <t>Sprint 15</t>
+  </si>
+  <si>
+    <t>Sprint 16</t>
+  </si>
+  <si>
+    <t>Sprint 17</t>
+  </si>
+  <si>
+    <t>Sprint 18</t>
+  </si>
+  <si>
+    <t>Sprint 19</t>
+  </si>
+  <si>
+    <t>Sprint 20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,9 +144,14 @@
       <family val="3"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -151,12 +177,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,25 +506,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755281A5-B63A-4AC1-AAE1-18F4017133B0}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -500,151 +535,456 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5">
+        <v>45546</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45560</v>
+      </c>
+      <c r="D2" s="5">
+        <v>45579</v>
+      </c>
+      <c r="E2" s="5">
+        <v>45590</v>
+      </c>
+      <c r="F2" s="5">
+        <v>45608</v>
+      </c>
+      <c r="G2" s="5">
+        <v>45623</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45624</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
+      <c r="L2" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="K3">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5">
+        <v>45561</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45575</v>
+      </c>
+      <c r="D3" s="5">
+        <v>45594</v>
+      </c>
+      <c r="E3" s="5">
+        <v>45607</v>
+      </c>
+      <c r="F3" s="5">
+        <v>45625</v>
+      </c>
+      <c r="G3" s="5">
+        <v>45638</v>
+      </c>
+      <c r="H3" s="5">
+        <v>45639</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="3">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3">
         <v>0</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="5">
+        <v>45576</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45590</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45609</v>
+      </c>
+      <c r="E4" s="5">
+        <v>45624</v>
+      </c>
+      <c r="F4" s="5">
+        <v>45642</v>
+      </c>
+      <c r="G4" s="5">
+        <v>45656</v>
+      </c>
+      <c r="H4" s="5">
+        <v>45657</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="3">
+        <v>10</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5">
+        <v>45593</v>
+      </c>
+      <c r="C5" s="5">
+        <v>45607</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45628</v>
+      </c>
+      <c r="E5" s="5">
+        <v>45639</v>
+      </c>
+      <c r="F5" s="5">
+        <v>45659</v>
+      </c>
+      <c r="G5" s="5">
+        <v>45672</v>
+      </c>
+      <c r="H5" s="5">
+        <v>45673</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="3">
+        <v>10</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="B6" s="5">
+        <v>45610</v>
+      </c>
+      <c r="C6" s="5">
+        <v>45624</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45643</v>
+      </c>
+      <c r="E6" s="5">
+        <v>45657</v>
+      </c>
+      <c r="F6" s="5">
+        <v>45674</v>
+      </c>
+      <c r="G6" s="5">
+        <v>45687</v>
+      </c>
+      <c r="H6" s="5">
+        <v>45688</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3">
+        <v>10</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5">
+        <v>45625</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45639</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45660</v>
+      </c>
+      <c r="E7" s="5">
+        <v>45673</v>
+      </c>
+      <c r="F7" s="5">
+        <v>45691</v>
+      </c>
+      <c r="G7" s="5">
+        <v>45702</v>
+      </c>
+      <c r="H7" s="5">
+        <v>45705</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="3">
+        <v>10</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5">
+        <v>45643</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45657</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45677</v>
+      </c>
+      <c r="E8" s="5">
+        <v>45688</v>
+      </c>
+      <c r="F8" s="5">
+        <v>45706</v>
+      </c>
+      <c r="G8" s="5">
+        <v>45719</v>
+      </c>
+      <c r="H8" s="5">
+        <v>45720</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J8" s="3">
+        <v>10</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="5">
+        <v>45659</v>
+      </c>
+      <c r="C9" s="5">
+        <v>45673</v>
+      </c>
+      <c r="D9" s="5">
+        <v>45692</v>
+      </c>
+      <c r="E9" s="5">
+        <v>45705</v>
+      </c>
+      <c r="F9" s="5">
+        <v>45721</v>
+      </c>
+      <c r="G9" s="5">
+        <v>45734</v>
+      </c>
+      <c r="H9" s="5">
+        <v>45735</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="3">
+        <v>10</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="5">
+        <v>45674</v>
+      </c>
+      <c r="C10" s="5">
+        <v>45688</v>
+      </c>
+      <c r="D10" s="5">
+        <v>45707</v>
+      </c>
+      <c r="E10" s="5">
+        <v>45720</v>
+      </c>
+      <c r="F10" s="5">
+        <v>45736</v>
+      </c>
+      <c r="G10" s="5">
+        <v>45749</v>
+      </c>
+      <c r="H10" s="5">
+        <v>45750</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="3">
+        <v>10</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="5">
+        <v>45691</v>
+      </c>
+      <c r="C11" s="5">
+        <v>45705</v>
+      </c>
+      <c r="D11" s="5">
+        <v>45722</v>
+      </c>
+      <c r="E11" s="5">
+        <v>45735</v>
+      </c>
+      <c r="F11" s="5">
+        <v>45751</v>
+      </c>
+      <c r="G11" s="5">
+        <v>45764</v>
+      </c>
+      <c r="H11" s="5">
+        <v>45765</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="3">
+        <v>10</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="5">
+        <v>45706</v>
+      </c>
+      <c r="C12" s="5">
+        <v>45720</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45737</v>
+      </c>
+      <c r="E12" s="5">
+        <v>45750</v>
+      </c>
+      <c r="F12" s="5">
+        <v>45768</v>
+      </c>
+      <c r="G12" s="5">
+        <v>45779</v>
+      </c>
+      <c r="H12" s="5">
+        <v>45782</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J4">
-        <v>10</v>
-      </c>
-      <c r="K4">
+      <c r="J12" s="3">
+        <v>10</v>
+      </c>
+      <c r="K12" s="3">
         <v>0</v>
       </c>
-      <c r="L4">
+      <c r="L12" s="4">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Desenvolvimento Graficos Issue Type e por Severity
</commit_message>
<xml_diff>
--- a/data/sprint_schedules.xlsx
+++ b/data/sprint_schedules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Python_Models2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B212BE8B-69EE-462B-95C5-BC66E0DF5367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DF997B-0444-43A5-A080-D3643A2BC3F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F5583670-12E1-4BD6-A5F2-68B02C1D08BA}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
         <v>45579</v>
       </c>
       <c r="E2" s="5">
-        <v>45590</v>
+        <v>45593</v>
       </c>
       <c r="F2" s="5">
         <v>45608</v>

</xml_diff>